<commit_message>
test case add emergency contact added
</commit_message>
<xml_diff>
--- a/test_data/orangehrm_data.xlsx
+++ b/test_data/orangehrm_data.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8633"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8633" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="VerifyAddEmployeeEnabled" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="VerifyAddEmergencyContact" sheetId="3" r:id="rId2"/>
+    <sheet name="VerifyAddEmployeeEnabled" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>${username}</t>
   </si>
@@ -104,6 +104,30 @@
   </si>
   <si>
     <t>KenE1002</t>
+  </si>
+  <si>
+    <t>${contact_name}</t>
+  </si>
+  <si>
+    <t>${relationship}</t>
+  </si>
+  <si>
+    <t>${homephone}</t>
+  </si>
+  <si>
+    <t>${mobilephone}</t>
+  </si>
+  <si>
+    <t>${workphone}</t>
+  </si>
+  <si>
+    <t>tony stark</t>
+  </si>
+  <si>
+    <t>friend</t>
+  </si>
+  <si>
+    <t>bala</t>
   </si>
 </sst>
 </file>
@@ -431,9 +455,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.9296875" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2">
+        <v>999999999</v>
+      </c>
+      <c r="F2">
+        <v>9876543210</v>
+      </c>
+      <c r="G2" s="3">
+        <v>9898989898</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3">
+        <v>999999999</v>
+      </c>
+      <c r="F3">
+        <v>9876543210</v>
+      </c>
+      <c r="G3" s="3">
+        <v>9898989898</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -576,30 +706,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
page object for add emergency and documentation for login page
</commit_message>
<xml_diff>
--- a/test_data/orangehrm_data.xlsx
+++ b/test_data/orangehrm_data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>${username}</t>
   </si>
@@ -121,13 +121,10 @@
     <t>${workphone}</t>
   </si>
   <si>
-    <t>tony stark</t>
-  </si>
-  <si>
     <t>friend</t>
   </si>
   <si>
-    <t>bala</t>
+    <t>tony starks</t>
   </si>
 </sst>
 </file>
@@ -467,10 +464,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -515,10 +512,10 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
         <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
       </c>
       <c r="E2">
         <v>999999999</v>
@@ -527,29 +524,6 @@
         <v>9876543210</v>
       </c>
       <c r="G2" s="3">
-        <v>9898989898</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3">
-        <v>999999999</v>
-      </c>
-      <c r="F3">
-        <v>9876543210</v>
-      </c>
-      <c r="G3" s="3">
         <v>9898989898</v>
       </c>
     </row>

</xml_diff>